<commit_message>
add changes to files
</commit_message>
<xml_diff>
--- a/Data/raw_excel/lovbio013b/PIGMENTS/icb_17042013_pig_extraits.xlsx
+++ b/Data/raw_excel/lovbio013b/PIGMENTS/icb_17042013_pig_extraits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="214" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,268 +13,273 @@
     <sheet name="Feuille3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="86">
   <si>
-    <t>Date of analysis</t>
-  </si>
-  <si>
-    <t>Ship</t>
-  </si>
-  <si>
-    <t>Cruise or Project</t>
-  </si>
-  <si>
-    <t>PI</t>
-  </si>
-  <si>
-    <t>Sampling date</t>
-  </si>
-  <si>
-    <t>Sampling time (TU)</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>CTD</t>
-  </si>
-  <si>
-    <t>Bottle</t>
-  </si>
-  <si>
-    <t>Sample code</t>
-  </si>
-  <si>
-    <t>Depth (m)</t>
-  </si>
-  <si>
-    <t>Filtered Vol (L)</t>
-  </si>
-  <si>
-    <t>Chlorophyll c3</t>
-  </si>
-  <si>
-    <t>Chlc3-QA</t>
-  </si>
-  <si>
-    <t>Chlorophyll c1+c2</t>
-  </si>
-  <si>
-    <t>Chlc2c1-QA</t>
-  </si>
-  <si>
-    <t>Sum Chlorophyllide a</t>
-  </si>
-  <si>
-    <t>Chlda-QA</t>
-  </si>
-  <si>
-    <t>Peridinin</t>
-  </si>
-  <si>
-    <t>Peri-QA</t>
-  </si>
-  <si>
-    <t>Sum Phaeophorbid a</t>
-  </si>
-  <si>
-    <t>Phda-QA</t>
-  </si>
-  <si>
-    <t>19'-Butanoyloxyfucoxanthin</t>
-  </si>
-  <si>
-    <t>But-QA</t>
-  </si>
-  <si>
-    <t>Fucoxanthin</t>
-  </si>
-  <si>
-    <t>Fuco-QA</t>
-  </si>
-  <si>
-    <t>Neoxanthin</t>
-  </si>
-  <si>
-    <t>Neo-QA</t>
-  </si>
-  <si>
-    <t>Prasinoxanthin</t>
-  </si>
-  <si>
-    <t>Pras-QA</t>
-  </si>
-  <si>
-    <t>Violaxanthin</t>
-  </si>
-  <si>
-    <t>Viola-QA</t>
-  </si>
-  <si>
-    <t>19'-Hexanoyloxyfucoxanthin</t>
-  </si>
-  <si>
-    <t>Hex-QA</t>
-  </si>
-  <si>
-    <t>Diadinoxanthin</t>
-  </si>
-  <si>
-    <t>Diadino-QA</t>
-  </si>
-  <si>
-    <t>Alloxanthin</t>
-  </si>
-  <si>
-    <t>Allo-QA</t>
-  </si>
-  <si>
-    <t>Diatoxanthin</t>
-  </si>
-  <si>
-    <t>Diato-QA</t>
-  </si>
-  <si>
-    <t>Zeaxanthin</t>
-  </si>
-  <si>
-    <t>Zea-QA</t>
-  </si>
-  <si>
-    <t>Lutein</t>
-  </si>
-  <si>
-    <t>Lut-QA</t>
-  </si>
-  <si>
-    <t>Bacteriochlorophyll a</t>
-  </si>
-  <si>
-    <t>Bchla-QA</t>
-  </si>
-  <si>
-    <t>Divinyl Chlorophyll b</t>
-  </si>
-  <si>
-    <t>DVChlb-QA</t>
-  </si>
-  <si>
-    <t>Chlorophyll b</t>
-  </si>
-  <si>
-    <t>Chlb-QA</t>
-  </si>
-  <si>
-    <t>Total Chlorophyll b</t>
-  </si>
-  <si>
-    <t>TChlb-QA</t>
-  </si>
-  <si>
-    <t>Divinyl Chlorophyll a</t>
-  </si>
-  <si>
-    <t>DVChla-QA</t>
-  </si>
-  <si>
-    <t>Chlorophyll a</t>
-  </si>
-  <si>
-    <t>Chla-QA</t>
-  </si>
-  <si>
-    <t>Total Chlorophyll a</t>
-  </si>
-  <si>
-    <t>Tchla-QA</t>
-  </si>
-  <si>
-    <t>sum Phaeophytin a</t>
-  </si>
-  <si>
-    <t>Phytna-QA</t>
-  </si>
-  <si>
-    <t>Sum carotenes</t>
-  </si>
-  <si>
-    <t>Tcar-QA</t>
-  </si>
-  <si>
-    <t>Observations</t>
-  </si>
-  <si>
-    <t>R/V Drofn</t>
-  </si>
-  <si>
-    <t>REY1</t>
-  </si>
-  <si>
-    <t>Claustre</t>
-  </si>
-  <si>
-    <t>17042013-1</t>
-  </si>
-  <si>
-    <t>170413-200</t>
-  </si>
-  <si>
-    <t>LOD</t>
-  </si>
-  <si>
-    <t>170413-160</t>
-  </si>
-  <si>
-    <t>170413-140</t>
-  </si>
-  <si>
-    <t>170413-120</t>
-  </si>
-  <si>
-    <t>170413-100</t>
-  </si>
-  <si>
-    <t>170413-080</t>
-  </si>
-  <si>
-    <t>170413-040</t>
-  </si>
-  <si>
-    <t>170413-020</t>
-  </si>
-  <si>
-    <t>170413-010</t>
-  </si>
-  <si>
-    <t>170413-005</t>
-  </si>
-  <si>
-    <t>17042013-2</t>
-  </si>
-  <si>
-    <t>prelevement 2h apres echantillonnage</t>
-  </si>
-  <si>
-    <t>170413-180</t>
-  </si>
-  <si>
-    <t>170413-150</t>
-  </si>
-  <si>
-    <t>170413-070</t>
-  </si>
-  <si>
-    <t>170413-030</t>
-  </si>
-  <si>
-    <t>170413-240</t>
+    <t xml:space="preserve">Date of analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruise or Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling time (TU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtered Vol (L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorophyll c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlc3-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorophyll c1+c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlc2c1-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum Chlorophyllide a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlda-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peridinin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peri-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum Phaeophorbid a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phda-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19'-Butanoyloxyfucoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">But-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fucoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuco-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neo-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prasinoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pras-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violaxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viola-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19'-Hexanoyloxyfucoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diadinoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diadino-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alloxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allo-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diatoxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diato-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeaxanthin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zea-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lutein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lut-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteriochlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bchla-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divinyl Chlorophyll b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVChlb-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorophyll b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlb-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Chlorophyll b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TChlb-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divinyl Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DVChla-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chla-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tchla-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum Phaeophytin a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phytna-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum carotenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tcar-QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R/V Drofn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claustre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17042013-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17042013-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prelevement 2h apres echantillonnage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170413-240</t>
   </si>
 </sst>
 </file>
@@ -282,30 +287,31 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YYYY" numFmtId="165"/>
-    <numFmt formatCode="HH:MM" numFmtId="166"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,7 +323,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -326,48 +332,59 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -379,15 +396,16 @@
   </sheetPr>
   <dimension ref="A1:BL21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="1:21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.85" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="35.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>41542</v>
       </c>
@@ -775,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>41542</v>
       </c>
@@ -969,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>41542</v>
       </c>
@@ -1163,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>41542</v>
       </c>
@@ -1357,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>41542</v>
       </c>
@@ -1551,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>41542</v>
       </c>
@@ -1745,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>41542</v>
       </c>
@@ -1939,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>41542</v>
       </c>
@@ -2133,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>41542</v>
       </c>
@@ -2327,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>41542</v>
       </c>
@@ -2521,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>41542</v>
       </c>
@@ -2544,7 +2562,7 @@
         <v>62.7247</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>-28.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>79</v>
@@ -2715,7 +2733,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>41542</v>
       </c>
@@ -2738,7 +2756,7 @@
         <v>62.7247</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>-27.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>79</v>
@@ -2909,7 +2927,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>41542</v>
       </c>
@@ -2932,7 +2950,7 @@
         <v>62.7247</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>-26.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>79</v>
@@ -3103,7 +3121,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>41542</v>
       </c>
@@ -3126,7 +3144,7 @@
         <v>62.7247</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>-25.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>79</v>
@@ -3297,7 +3315,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>41542</v>
       </c>
@@ -3320,7 +3338,7 @@
         <v>62.7247</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>-24.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>79</v>
@@ -3491,7 +3509,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <v>41542</v>
       </c>
@@ -3514,7 +3532,7 @@
         <v>62.7247</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>-23.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>79</v>
@@ -3685,7 +3703,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
         <v>41542</v>
       </c>
@@ -3708,7 +3726,7 @@
         <v>62.7247</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>-22.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>79</v>
@@ -3879,7 +3897,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
         <v>41542</v>
       </c>
@@ -3902,7 +3920,7 @@
         <v>62.7247</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>-21.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>79</v>
@@ -4073,7 +4091,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
         <v>41542</v>
       </c>
@@ -4267,7 +4285,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
         <v>41542</v>
       </c>
@@ -4290,7 +4308,7 @@
         <v>62.7247</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>-29.6262</v>
+        <v>-20.6262</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>79</v>
@@ -4464,7 +4482,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -4479,17 +4497,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -4504,17 +4523,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>